<commit_message>
Fixed absolute hex address in chart
</commit_message>
<xml_diff>
--- a/Chart.xlsx
+++ b/Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\links3\Google Drive\School\2019 Spring\Telecom\Homework\3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\links3\Google Drive\School\2019 Spring\Telecom\Homework\3\TelecomAssignment2Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Capture #</t>
   </si>
@@ -95,20 +95,26 @@
     <t>Reltive Decimal</t>
   </si>
   <si>
-    <t>Reletive Decimal</t>
-  </si>
-  <si>
     <t>8FA1AFB2</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>0x00000011 FIN, ACK</t>
+  </si>
+  <si>
+    <t>0D618385</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,13 +122,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -186,8 +216,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -202,26 +234,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,10 +604,10 @@
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
@@ -589,10 +623,10 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11"/>
+      <c r="M1" s="6"/>
       <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
@@ -614,697 +648,712 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>922</v>
+      </c>
+      <c r="B3" s="7">
+        <v>54762</v>
+      </c>
+      <c r="C3" s="7">
+        <v>443</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>922</v>
-      </c>
-      <c r="B3" s="6">
-        <v>54762</v>
-      </c>
-      <c r="C3" s="6">
-        <v>443</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>0</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="7">
         <v>32</v>
       </c>
-      <c r="I3" s="6">
-        <v>20</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="I3" s="7">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7">
         <v>52</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="7">
         <f>J3-I3-H3</f>
         <v>0</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="7">
         <v>3582</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="7">
+      <c r="M3" s="7">
+        <f>HEX2DEC(L3)</f>
+        <v>13698</v>
+      </c>
+      <c r="N3" s="8">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>928</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>443</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>54762</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="str">
+      <c r="E4" s="7" t="str">
         <f>DEC2HEX(HEX2DEC(E3)+F4)</f>
         <v>8FA1AFB2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>0</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <v>32</v>
       </c>
-      <c r="I4" s="6">
-        <v>20</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="I4" s="7">
+        <v>20</v>
+      </c>
+      <c r="J4" s="7">
         <v>52</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="7">
         <f t="shared" ref="K4:K17" si="0">J4-I4-H4</f>
         <v>0</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="7">
         <v>0</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="6">
+      <c r="M4" s="7">
+        <f t="shared" ref="M4:M17" si="1">HEX2DEC(L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>929</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>54762</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>443</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="str">
-        <f t="shared" ref="E5:E16" si="1">DEC2HEX(HEX2DEC(E4)+F5)</f>
+      <c r="E5" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E4)+F5)</f>
         <v>8FA1AFB3</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>1</v>
       </c>
-      <c r="H5" s="6">
-        <v>20</v>
-      </c>
-      <c r="I5" s="6">
-        <v>20</v>
-      </c>
-      <c r="J5" s="6">
+      <c r="H5" s="7">
+        <v>20</v>
+      </c>
+      <c r="I5" s="7">
+        <v>20</v>
+      </c>
+      <c r="J5" s="7">
         <v>40</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="7">
         <v>3583</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="M5" s="7">
+        <f t="shared" si="1"/>
+        <v>13699</v>
+      </c>
+      <c r="N5" s="7">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>930</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>54762</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>443</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA1AFB4</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E6" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F6)</f>
+        <v>8FA1AFB3</v>
+      </c>
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="H6" s="6">
-        <v>20</v>
-      </c>
-      <c r="I6" s="6">
-        <v>20</v>
-      </c>
-      <c r="J6" s="6">
+      <c r="H6" s="7">
+        <v>20</v>
+      </c>
+      <c r="I6" s="7">
+        <v>20</v>
+      </c>
+      <c r="J6" s="7">
         <v>557</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="7">
         <f t="shared" si="0"/>
         <v>517</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="7">
         <v>3584</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="6">
+      <c r="M6" s="7">
+        <f t="shared" si="1"/>
+        <v>13700</v>
+      </c>
+      <c r="N6" s="7">
         <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>935</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>443</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>54762</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA1AFB5</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F7)</f>
+        <v>8FA1AFB3</v>
+      </c>
+      <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <v>518</v>
       </c>
-      <c r="H7" s="6">
-        <v>20</v>
-      </c>
-      <c r="I7" s="6">
-        <v>20</v>
-      </c>
-      <c r="J7" s="6">
+      <c r="H7" s="7">
+        <v>20</v>
+      </c>
+      <c r="I7" s="7">
+        <v>20</v>
+      </c>
+      <c r="J7" s="7">
         <v>40</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="7">
         <v>6705</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="8">
+      <c r="M7" s="7">
+        <f t="shared" si="1"/>
+        <v>26373</v>
+      </c>
+      <c r="N7" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>936</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>443</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>54762</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="str">
-        <f>DEC2HEX(HEX2DEC(E7)+F8)</f>
-        <v>8FA1AFB6</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="E8" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F8)</f>
+        <v>8FA1AFB3</v>
+      </c>
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="7">
         <v>518</v>
       </c>
-      <c r="H8" s="6">
-        <v>20</v>
-      </c>
-      <c r="I8" s="6">
-        <v>20</v>
-      </c>
-      <c r="J8" s="6">
+      <c r="H8" s="7">
+        <v>20</v>
+      </c>
+      <c r="I8" s="7">
+        <v>20</v>
+      </c>
+      <c r="J8" s="7">
         <v>1500</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="7">
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="7">
         <v>6706</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="8">
+      <c r="M8" s="7">
+        <f t="shared" si="1"/>
+        <v>26374</v>
+      </c>
+      <c r="N8" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>937</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>443</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>54762</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA1B56B</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="7" t="str">
+        <f t="shared" ref="E5:E16" si="2">DEC2HEX(HEX2DEC(E8)+F9)</f>
+        <v>8FA1B568</v>
+      </c>
+      <c r="F9" s="7">
         <v>1461</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="7">
         <v>518</v>
       </c>
-      <c r="H9" s="6">
-        <v>20</v>
-      </c>
-      <c r="I9" s="6">
-        <v>20</v>
-      </c>
-      <c r="J9" s="6">
+      <c r="H9" s="7">
+        <v>20</v>
+      </c>
+      <c r="I9" s="7">
+        <v>20</v>
+      </c>
+      <c r="J9" s="7">
         <v>1500</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="7">
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="7">
         <v>6707</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="8">
+      <c r="M9" s="7">
+        <f t="shared" si="1"/>
+        <v>26375</v>
+      </c>
+      <c r="N9" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>938</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>443</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>54762</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA1B771</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="E10" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F10)</f>
+        <v>8FA1B1B8</v>
+      </c>
+      <c r="F10" s="7">
         <v>518</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="7">
         <v>2921</v>
       </c>
-      <c r="H10" s="6">
-        <v>20</v>
-      </c>
-      <c r="I10" s="6">
-        <v>20</v>
-      </c>
-      <c r="J10" s="6">
+      <c r="H10" s="7">
+        <v>20</v>
+      </c>
+      <c r="I10" s="7">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7">
         <v>40</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="7">
         <v>3585</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="8">
+      <c r="M10" s="7">
+        <f t="shared" si="1"/>
+        <v>13701</v>
+      </c>
+      <c r="N10" s="7">
         <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="7">
         <v>939</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>443</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>54762</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA1C2DA</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="E11" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F11)</f>
+        <v>8FA1BB1B</v>
+      </c>
+      <c r="F11" s="7">
         <v>2921</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="7">
         <v>518</v>
       </c>
-      <c r="H11" s="6">
-        <v>20</v>
-      </c>
-      <c r="I11" s="6">
-        <v>20</v>
-      </c>
-      <c r="J11" s="6">
+      <c r="H11" s="7">
+        <v>20</v>
+      </c>
+      <c r="I11" s="7">
+        <v>20</v>
+      </c>
+      <c r="J11" s="7">
         <v>1500</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="7">
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="7">
         <v>6708</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="8">
+      <c r="M11" s="7">
+        <f t="shared" si="1"/>
+        <v>26376</v>
+      </c>
+      <c r="N11" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <v>940</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="7">
         <v>443</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>54762</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA1D3F7</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="E12" s="7" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F12)</f>
+        <v>8FA1C0CF</v>
+      </c>
+      <c r="F12" s="7">
         <v>4381</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="7">
         <v>518</v>
       </c>
-      <c r="H12" s="6">
-        <v>20</v>
-      </c>
-      <c r="I12" s="6">
-        <v>20</v>
-      </c>
-      <c r="J12" s="6">
+      <c r="H12" s="7">
+        <v>20</v>
+      </c>
+      <c r="I12" s="7">
+        <v>20</v>
+      </c>
+      <c r="J12" s="7">
         <v>600</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="7">
         <f t="shared" si="0"/>
         <v>560</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="7">
         <v>6709</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="8">
+      <c r="M12" s="7">
+        <f t="shared" si="1"/>
+        <v>26377</v>
+      </c>
+      <c r="N12" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="9">
         <v>978</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="9">
         <v>443</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="9">
         <v>54762</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA24592</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="E13" s="9" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F13)</f>
+        <v>8FA2214D</v>
+      </c>
+      <c r="F13" s="9">
         <v>29083</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="9">
         <v>1047</v>
       </c>
-      <c r="H13" s="6">
-        <v>20</v>
-      </c>
-      <c r="I13" s="6">
-        <v>20</v>
-      </c>
-      <c r="J13" s="6">
+      <c r="H13" s="9">
+        <v>20</v>
+      </c>
+      <c r="I13" s="9">
+        <v>20</v>
+      </c>
+      <c r="J13" s="9">
         <v>1500</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="9">
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="8">
+      <c r="M13" s="9">
+        <f t="shared" si="1"/>
+        <v>26395</v>
+      </c>
+      <c r="N13" s="9">
         <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="9">
         <v>979</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="9">
         <v>54762</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="9">
         <v>443</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA249A9</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="E14" s="9" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F14)</f>
+        <v>8FA1B3C9</v>
+      </c>
+      <c r="F14" s="9">
         <v>1047</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="9">
         <v>29083</v>
       </c>
-      <c r="H14" s="6">
-        <v>20</v>
-      </c>
-      <c r="I14" s="6">
-        <v>20</v>
-      </c>
-      <c r="J14" s="6">
+      <c r="H14" s="9">
+        <v>20</v>
+      </c>
+      <c r="I14" s="9">
+        <v>20</v>
+      </c>
+      <c r="J14" s="9">
         <v>40</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="9">
         <v>3591</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="8">
+      <c r="M14" s="9">
+        <f t="shared" si="1"/>
+        <v>13713</v>
+      </c>
+      <c r="N14" s="9">
         <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="9">
         <v>980</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="9">
         <v>443</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="9">
         <v>54762</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA2BB44</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="E15" s="9" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F15)</f>
+        <v>8FA2214D</v>
+      </c>
+      <c r="F15" s="9">
         <v>29083</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="9">
         <v>1047</v>
       </c>
-      <c r="H15" s="6">
-        <v>20</v>
-      </c>
-      <c r="I15" s="6">
-        <v>20</v>
-      </c>
-      <c r="J15" s="6">
+      <c r="H15" s="9">
+        <v>20</v>
+      </c>
+      <c r="I15" s="9">
+        <v>20</v>
+      </c>
+      <c r="J15" s="9">
         <v>1500</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="9">
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="8">
+      <c r="M15" s="9">
+        <f t="shared" si="1"/>
+        <v>26396</v>
+      </c>
+      <c r="N15" s="9">
         <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="9">
         <v>981</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="9">
         <v>443</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="9">
         <v>54762</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>8FA33293</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="E16" s="9" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F16)</f>
+        <v>8FA22701</v>
+      </c>
+      <c r="F16" s="9">
         <v>30543</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="9">
         <v>1047</v>
       </c>
-      <c r="H16" s="6">
-        <v>20</v>
-      </c>
-      <c r="I16" s="6">
-        <v>20</v>
-      </c>
-      <c r="J16" s="6">
+      <c r="H16" s="9">
+        <v>20</v>
+      </c>
+      <c r="I16" s="9">
+        <v>20</v>
+      </c>
+      <c r="J16" s="9">
         <v>1319</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="9">
         <f t="shared" si="0"/>
         <v>1279</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="8">
+      <c r="M16" s="9">
+        <f t="shared" si="1"/>
+        <v>26397</v>
+      </c>
+      <c r="N16" s="9">
         <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="10">
         <v>982</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="10">
         <v>54762</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="10">
         <v>443</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(E16)+F17)</f>
-        <v>8FA336AA</v>
-      </c>
-      <c r="F17" s="9">
+      <c r="E17" s="10" t="str">
+        <f>DEC2HEX(HEX2DEC(E3)+F17)</f>
+        <v>8FA1B3C9</v>
+      </c>
+      <c r="F17" s="10">
         <v>1047</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="10">
         <v>31822</v>
       </c>
-      <c r="H17" s="9">
-        <v>20</v>
-      </c>
-      <c r="I17" s="9">
-        <v>20</v>
-      </c>
-      <c r="J17" s="9">
+      <c r="H17" s="10">
+        <v>20</v>
+      </c>
+      <c r="I17" s="10">
+        <v>20</v>
+      </c>
+      <c r="J17" s="10">
         <v>40</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="10">
         <v>3592</v>
       </c>
-      <c r="M17" s="9" t="s">
-        <v>23</v>
+      <c r="M17" s="10">
+        <f t="shared" si="1"/>
+        <v>13714</v>
       </c>
       <c r="N17" s="10">
         <v>128</v>
@@ -1327,20 +1376,48 @@
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="2"/>
+      <c r="A19" s="11">
+        <v>4592</v>
+      </c>
+      <c r="B19" s="11">
+        <v>54764</v>
+      </c>
+      <c r="C19" s="11">
+        <v>443</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="11">
+        <v>569</v>
+      </c>
+      <c r="G19" s="11">
+        <v>138</v>
+      </c>
+      <c r="H19" s="11">
+        <v>20</v>
+      </c>
+      <c r="I19" s="11">
+        <v>20</v>
+      </c>
+      <c r="J19" s="11">
+        <v>40</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11">
+        <v>589</v>
+      </c>
+      <c r="M19" s="11">
+        <v>1417</v>
+      </c>
+      <c r="N19" s="11">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>

</xml_diff>